<commit_message>
New file for Jessica's data
</commit_message>
<xml_diff>
--- a/DLS_Plots/20231016_DLSData.xlsx
+++ b/DLS_Plots/20231016_DLSData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryellewright/Documents/Kumar-Biomaterials-Lab/DLS_Plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3E1345-BEB7-6244-A78B-7CDEA1BAB824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF27EC4E-F801-D047-89E9-ADE4C3828304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9440" yWindow="2340" windowWidth="14020" windowHeight="11240" xr2:uid="{107BFF65-5878-EC4C-9CA0-44FBC9A7FCCB}"/>
+    <workbookView xWindow="12380" yWindow="1920" windowWidth="14020" windowHeight="11240" xr2:uid="{107BFF65-5878-EC4C-9CA0-44FBC9A7FCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Polymer</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Effective Diameter Avg. (nm)</t>
   </si>
   <si>
-    <t>Std</t>
-  </si>
-  <si>
     <t>DMA G2</t>
   </si>
   <si>
@@ -70,6 +67,15 @@
   </si>
   <si>
     <t>DMA B2</t>
+  </si>
+  <si>
+    <t>PDI</t>
+  </si>
+  <si>
+    <t>Std PDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Std Diam. </t>
   </si>
 </sst>
 </file>
@@ -261,105 +267,168 @@
           <cell r="G2">
             <v>130.05000000000001</v>
           </cell>
+          <cell r="H2">
+            <v>0.18099999999999999</v>
+          </cell>
         </row>
         <row r="3">
           <cell r="G3">
             <v>119.81</v>
           </cell>
+          <cell r="H3">
+            <v>0.183</v>
+          </cell>
         </row>
         <row r="4">
           <cell r="G4">
             <v>127.34</v>
           </cell>
+          <cell r="H4">
+            <v>0.17199999999999999</v>
+          </cell>
         </row>
         <row r="5">
           <cell r="G5">
             <v>140.63</v>
           </cell>
+          <cell r="H5">
+            <v>0.185</v>
+          </cell>
         </row>
         <row r="6">
           <cell r="G6">
             <v>148.01</v>
           </cell>
+          <cell r="H6">
+            <v>0.156</v>
+          </cell>
         </row>
         <row r="7">
           <cell r="G7">
             <v>141.15</v>
           </cell>
+          <cell r="H7">
+            <v>0.17399999999999999</v>
+          </cell>
         </row>
         <row r="8">
           <cell r="G8">
             <v>114.19</v>
           </cell>
+          <cell r="H8">
+            <v>0.19600000000000001</v>
+          </cell>
         </row>
         <row r="9">
           <cell r="G9">
             <v>115.78</v>
           </cell>
+          <cell r="H9">
+            <v>0.20599999999999999</v>
+          </cell>
         </row>
         <row r="10">
           <cell r="G10">
             <v>111.11</v>
           </cell>
+          <cell r="H10">
+            <v>0.20699999999999999</v>
+          </cell>
         </row>
         <row r="11">
           <cell r="G11">
             <v>113.64</v>
           </cell>
+          <cell r="H11">
+            <v>0.23200000000000001</v>
+          </cell>
         </row>
         <row r="12">
           <cell r="G12">
             <v>113.48</v>
           </cell>
+          <cell r="H12">
+            <v>0.23699999999999999</v>
+          </cell>
         </row>
         <row r="13">
           <cell r="G13">
             <v>115.54</v>
           </cell>
+          <cell r="H13">
+            <v>0.19700000000000001</v>
+          </cell>
         </row>
         <row r="14">
           <cell r="G14">
             <v>111.1</v>
           </cell>
+          <cell r="H14">
+            <v>0.19700000000000001</v>
+          </cell>
         </row>
         <row r="15">
           <cell r="G15">
             <v>115.39</v>
           </cell>
+          <cell r="H15">
+            <v>0.18</v>
+          </cell>
         </row>
         <row r="16">
           <cell r="G16">
             <v>116.73</v>
           </cell>
+          <cell r="H16">
+            <v>0.18099999999999999</v>
+          </cell>
         </row>
         <row r="17">
           <cell r="G17">
             <v>113.68</v>
           </cell>
+          <cell r="H17">
+            <v>0.158</v>
+          </cell>
         </row>
         <row r="18">
           <cell r="G18">
             <v>114.71</v>
           </cell>
+          <cell r="H18">
+            <v>0.128</v>
+          </cell>
         </row>
         <row r="19">
           <cell r="G19">
             <v>117.95</v>
           </cell>
+          <cell r="H19">
+            <v>6.9000000000000006E-2</v>
+          </cell>
         </row>
         <row r="20">
           <cell r="G20">
             <v>119.11</v>
           </cell>
+          <cell r="H20">
+            <v>5.3999999999999999E-2</v>
+          </cell>
         </row>
         <row r="21">
           <cell r="G21">
             <v>115.05</v>
           </cell>
+          <cell r="H21">
+            <v>0.158</v>
+          </cell>
         </row>
         <row r="22">
           <cell r="G22">
             <v>121.02</v>
+          </cell>
+          <cell r="H22">
+            <v>0.16700000000000001</v>
           </cell>
         </row>
       </sheetData>
@@ -665,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A67EDDD-4556-584C-82BA-9B5528297131}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A18"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,7 +746,7 @@
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -685,12 +754,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <f>AVERAGE('[1]20231016_DLSData'!$G$2:$G$4)</f>
@@ -700,10 +775,18 @@
         <f>STDEV('[2]20231016_DLSData'!$G$2:$G$4)</f>
         <v>5.3056981947085315</v>
       </c>
+      <c r="D2">
+        <f>AVERAGE('[2]20231016_DLSData'!$H$2:$H$4)</f>
+        <v>0.17866666666666667</v>
+      </c>
+      <c r="E2">
+        <f>STDEV('[2]20231016_DLSData'!$H$2:$H$4)</f>
+        <v>5.8594652770823201E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <f>AVERAGE('[1]20231016_DLSData'!$G$5:$G$7)</f>
@@ -713,10 +796,18 @@
         <f>STDEV('[2]20231016_DLSData'!$G$5:$G$7)</f>
         <v>4.1189480857778831</v>
       </c>
+      <c r="D3">
+        <f>AVERAGE('[2]20231016_DLSData'!$H$5:$H$7)</f>
+        <v>0.17166666666666663</v>
+      </c>
+      <c r="E3">
+        <f>STDEV('[2]20231016_DLSData'!$H$5:$H$7)</f>
+        <v>1.4640127503998497E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <f>AVERAGE('[1]20231016_DLSData'!$G$8:$G$10)</f>
@@ -726,10 +817,18 @@
         <f>STDEV('[2]20231016_DLSData'!$G$8:$G$10)</f>
         <v>2.3742858575439767</v>
       </c>
+      <c r="D4">
+        <f>AVERAGE('[2]20231016_DLSData'!$H$8:$H$10)</f>
+        <v>0.20299999999999999</v>
+      </c>
+      <c r="E4">
+        <f>STDEV('[2]20231016_DLSData'!$H$8:$H$10)</f>
+        <v>6.0827625302982092E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <f>AVERAGE('[1]20231016_DLSData'!$G$11:$G$13)</f>
@@ -739,10 +838,18 @@
         <f>STDEV('[2]20231016_DLSData'!$G$11:$G$13)</f>
         <v>1.1459493880621452</v>
       </c>
+      <c r="D5">
+        <f>AVERAGE('[2]20231016_DLSData'!$H$11:$H$13)</f>
+        <v>0.22199999999999998</v>
+      </c>
+      <c r="E5">
+        <f>STDEV('[2]20231016_DLSData'!$H$11:$H$13)</f>
+        <v>2.1794494717703363E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <f>AVERAGE('[1]20231016_DLSData'!$G$14:$G$16)</f>
@@ -752,10 +859,18 @@
         <f>STDEV('[2]20231016_DLSData'!$G$14:$G$16)</f>
         <v>2.9409918961692778</v>
       </c>
+      <c r="D6">
+        <f>AVERAGE('[2]20231016_DLSData'!$H$14:$H$16)</f>
+        <v>0.18600000000000003</v>
+      </c>
+      <c r="E6">
+        <f>STDEV('[2]20231016_DLSData'!$H$14:$H$16)</f>
+        <v>9.5393920141694649E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <f>AVERAGE('[1]20231016_DLSData'!$G$17:$G$19)</f>
@@ -765,10 +880,18 @@
         <f>STDEV('[2]20231016_DLSData'!$G$17:$G$19)</f>
         <v>2.2282803533966127</v>
       </c>
+      <c r="D7">
+        <f>AVERAGE('[2]20231016_DLSData'!$H$17:$H$19)</f>
+        <v>0.11833333333333335</v>
+      </c>
+      <c r="E7">
+        <f>STDEV('[2]20231016_DLSData'!$H$17:$H$19)</f>
+        <v>4.5280606591932129E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <f>AVERAGE('[1]20231016_DLSData'!$G$20:$G$22)</f>
@@ -777,6 +900,14 @@
       <c r="C8">
         <f>STDEV('[2]20231016_DLSData'!$G$20:$G$22)</f>
         <v>3.0488413099624143</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE('[2]20231016_DLSData'!$H$20:$H$22)</f>
+        <v>0.12633333333333333</v>
+      </c>
+      <c r="E8">
+        <f>STDEV('[2]20231016_DLSData'!$H$20:$H$22)</f>
+        <v>6.2803927690339031E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>